<commit_message>
final integration with spring security
</commit_message>
<xml_diff>
--- a/sql/INDO_CMS_TEMPLATE_QUERY.xlsx
+++ b/sql/INDO_CMS_TEMPLATE_QUERY.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="122">
   <si>
     <t xml:space="preserve">row_id</t>
   </si>
@@ -177,6 +177,12 @@
   </si>
   <si>
     <t xml:space="preserve">INDO_CMS_MENU_PERMISSION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAN VIEW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">can_view</t>
   </si>
   <si>
     <t xml:space="preserve">CAN INSERT</t>
@@ -477,10 +483,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P57"/>
+  <dimension ref="A1:P58"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+      <selection pane="topLeft" activeCell="P26" activeCellId="0" sqref="P26:P34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1563,7 +1569,7 @@
         <v>16</v>
       </c>
       <c r="G28" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H28" s="0" t="n">
         <v>0</v>
@@ -1579,7 +1585,7 @@
       </c>
       <c r="M28" s="0" t="str">
         <f aca="false">"('"&amp;B28&amp;"','"&amp;C28&amp;"','"&amp;D28&amp;"','"&amp;E28&amp;"','"&amp;F28&amp;"','"&amp;G28&amp;"','"&amp;H28&amp;"','"&amp;I28&amp;"','"&amp;J28&amp;"','"&amp;K28&amp;"');"</f>
-        <v>('INDO_CMS_MENU_PERMISSION','ROLE ID','role_id','role_id','STRING','2','0','1','1','1');</v>
+        <v>('INDO_CMS_MENU_PERMISSION','ROLE ID','role_id','role_id','STRING','3','0','1','1','1');</v>
       </c>
       <c r="N28" s="0" t="str">
         <f aca="false">"INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES"</f>
@@ -1587,7 +1593,7 @@
       </c>
       <c r="P28" s="0" t="str">
         <f aca="false">N28&amp;M28</f>
-        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_MENU_PERMISSION','ROLE ID','role_id','role_id','STRING','2','0','1','1','1');</v>
+        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_MENU_PERMISSION','ROLE ID','role_id','role_id','STRING','3','0','1','1','1');</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1607,7 +1613,7 @@
         <v>16</v>
       </c>
       <c r="G29" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H29" s="0" t="n">
         <v>0</v>
@@ -1623,7 +1629,7 @@
       </c>
       <c r="M29" s="0" t="str">
         <f aca="false">"('"&amp;B29&amp;"','"&amp;C29&amp;"','"&amp;D29&amp;"','"&amp;E29&amp;"','"&amp;F29&amp;"','"&amp;G29&amp;"','"&amp;H29&amp;"','"&amp;I29&amp;"','"&amp;J29&amp;"','"&amp;K29&amp;"');"</f>
-        <v>('INDO_CMS_MENU_PERMISSION','CAN INSERT','can_insert','can_insert','STRING','3','0','1','1','1');</v>
+        <v>('INDO_CMS_MENU_PERMISSION','CAN VIEW','can_view','can_view','STRING','4','0','1','1','1');</v>
       </c>
       <c r="N29" s="0" t="str">
         <f aca="false">"INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES"</f>
@@ -1631,7 +1637,7 @@
       </c>
       <c r="P29" s="0" t="str">
         <f aca="false">N29&amp;M29</f>
-        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_MENU_PERMISSION','CAN INSERT','can_insert','can_insert','STRING','3','0','1','1','1');</v>
+        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_MENU_PERMISSION','CAN VIEW','can_view','can_view','STRING','4','0','1','1','1');</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1651,7 +1657,7 @@
         <v>16</v>
       </c>
       <c r="G30" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H30" s="0" t="n">
         <v>0</v>
@@ -1667,7 +1673,7 @@
       </c>
       <c r="M30" s="0" t="str">
         <f aca="false">"('"&amp;B30&amp;"','"&amp;C30&amp;"','"&amp;D30&amp;"','"&amp;E30&amp;"','"&amp;F30&amp;"','"&amp;G30&amp;"','"&amp;H30&amp;"','"&amp;I30&amp;"','"&amp;J30&amp;"','"&amp;K30&amp;"');"</f>
-        <v>('INDO_CMS_MENU_PERMISSION','CAN UPDATE','can_update','can_update','STRING','4','0','1','1','1');</v>
+        <v>('INDO_CMS_MENU_PERMISSION','CAN INSERT','can_insert','can_insert','STRING','5','0','1','1','1');</v>
       </c>
       <c r="N30" s="0" t="str">
         <f aca="false">"INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES"</f>
@@ -1675,7 +1681,7 @@
       </c>
       <c r="P30" s="0" t="str">
         <f aca="false">N30&amp;M30</f>
-        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_MENU_PERMISSION','CAN UPDATE','can_update','can_update','STRING','4','0','1','1','1');</v>
+        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_MENU_PERMISSION','CAN INSERT','can_insert','can_insert','STRING','5','0','1','1','1');</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1695,7 +1701,7 @@
         <v>16</v>
       </c>
       <c r="G31" s="0" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H31" s="0" t="n">
         <v>0</v>
@@ -1711,7 +1717,7 @@
       </c>
       <c r="M31" s="0" t="str">
         <f aca="false">"('"&amp;B31&amp;"','"&amp;C31&amp;"','"&amp;D31&amp;"','"&amp;E31&amp;"','"&amp;F31&amp;"','"&amp;G31&amp;"','"&amp;H31&amp;"','"&amp;I31&amp;"','"&amp;J31&amp;"','"&amp;K31&amp;"');"</f>
-        <v>('INDO_CMS_MENU_PERMISSION','CAN DELETE','can_delete','can_delete','STRING','5','0','1','1','1');</v>
+        <v>('INDO_CMS_MENU_PERMISSION','CAN UPDATE','can_update','can_update','STRING','6','0','1','1','1');</v>
       </c>
       <c r="N31" s="0" t="str">
         <f aca="false">"INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES"</f>
@@ -1719,7 +1725,7 @@
       </c>
       <c r="P31" s="0" t="str">
         <f aca="false">N31&amp;M31</f>
-        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_MENU_PERMISSION','CAN DELETE','can_delete','can_delete','STRING','5','0','1','1','1');</v>
+        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_MENU_PERMISSION','CAN UPDATE','can_update','can_update','STRING','6','0','1','1','1');</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1739,7 +1745,7 @@
         <v>16</v>
       </c>
       <c r="G32" s="0" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H32" s="0" t="n">
         <v>0</v>
@@ -1755,7 +1761,7 @@
       </c>
       <c r="M32" s="0" t="str">
         <f aca="false">"('"&amp;B32&amp;"','"&amp;C32&amp;"','"&amp;D32&amp;"','"&amp;E32&amp;"','"&amp;F32&amp;"','"&amp;G32&amp;"','"&amp;H32&amp;"','"&amp;I32&amp;"','"&amp;J32&amp;"','"&amp;K32&amp;"');"</f>
-        <v>('INDO_CMS_MENU_PERMISSION','CAN EXPORT','can_export','can_export','STRING','6','0','1','1','1');</v>
+        <v>('INDO_CMS_MENU_PERMISSION','CAN DELETE','can_delete','can_delete','STRING','7','0','1','1','1');</v>
       </c>
       <c r="N32" s="0" t="str">
         <f aca="false">"INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES"</f>
@@ -1763,7 +1769,7 @@
       </c>
       <c r="P32" s="0" t="str">
         <f aca="false">N32&amp;M32</f>
-        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_MENU_PERMISSION','CAN EXPORT','can_export','can_export','STRING','6','0','1','1','1');</v>
+        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_MENU_PERMISSION','CAN DELETE','can_delete','can_delete','STRING','7','0','1','1','1');</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1783,7 +1789,7 @@
         <v>16</v>
       </c>
       <c r="G33" s="0" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H33" s="0" t="n">
         <v>0</v>
@@ -1799,7 +1805,7 @@
       </c>
       <c r="M33" s="0" t="str">
         <f aca="false">"('"&amp;B33&amp;"','"&amp;C33&amp;"','"&amp;D33&amp;"','"&amp;E33&amp;"','"&amp;F33&amp;"','"&amp;G33&amp;"','"&amp;H33&amp;"','"&amp;I33&amp;"','"&amp;J33&amp;"','"&amp;K33&amp;"');"</f>
-        <v>('INDO_CMS_MENU_PERMISSION','CAN IMPORT','can_import','can_import','STRING','7','0','1','1','1');</v>
+        <v>('INDO_CMS_MENU_PERMISSION','CAN EXPORT','can_export','can_export','STRING','8','0','1','1','1');</v>
       </c>
       <c r="N33" s="0" t="str">
         <f aca="false">"INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES"</f>
@@ -1807,87 +1813,87 @@
       </c>
       <c r="P33" s="0" t="str">
         <f aca="false">N33&amp;M33</f>
-        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_MENU_PERMISSION','CAN IMPORT','can_import','can_import','STRING','7','0','1','1','1');</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="0" t="s">
+        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_MENU_PERMISSION','CAN EXPORT','can_export','can_export','STRING','8','0','1','1','1');</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="C34" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="C35" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D35" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="E35" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="F35" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G35" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H35" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I35" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J35" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K35" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M35" s="0" t="str">
-        <f aca="false">"('"&amp;B35&amp;"','"&amp;C35&amp;"','"&amp;D35&amp;"','"&amp;E35&amp;"','"&amp;F35&amp;"','"&amp;G35&amp;"','"&amp;H35&amp;"','"&amp;I35&amp;"','"&amp;J35&amp;"','"&amp;K35&amp;"');"</f>
-        <v>('INDO_CMS_TEMPLATE_HEADER','ROW ID','row_id','row_id','INTEGER','1','1','1','0','0');</v>
-      </c>
-      <c r="N35" s="0" t="str">
-        <f aca="false">"INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES"</f>
-        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES</v>
-      </c>
-      <c r="P35" s="0" t="str">
-        <f aca="false">N35&amp;M35</f>
-        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_TEMPLATE_HEADER','ROW ID','row_id','row_id','INTEGER','1','1','1','0','0');</v>
+      <c r="D34" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G34" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="H34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M34" s="0" t="str">
+        <f aca="false">"('"&amp;B34&amp;"','"&amp;C34&amp;"','"&amp;D34&amp;"','"&amp;E34&amp;"','"&amp;F34&amp;"','"&amp;G34&amp;"','"&amp;H34&amp;"','"&amp;I34&amp;"','"&amp;J34&amp;"','"&amp;K34&amp;"');"</f>
+        <v>('INDO_CMS_MENU_PERMISSION','CAN IMPORT','can_import','can_import','STRING','9','0','1','1','1');</v>
+      </c>
+      <c r="N34" s="0" t="str">
+        <f aca="false">"INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES"</f>
+        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES</v>
+      </c>
+      <c r="P34" s="0" t="str">
+        <f aca="false">N34&amp;M34</f>
+        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_MENU_PERMISSION','CAN IMPORT','can_import','can_import','STRING','9','0','1','1','1');</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>63</v>
+        <v>12</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G36" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H36" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I36" s="0" t="n">
         <v>1</v>
       </c>
       <c r="J36" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K36" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M36" s="0" t="str">
         <f aca="false">"('"&amp;B36&amp;"','"&amp;C36&amp;"','"&amp;D36&amp;"','"&amp;E36&amp;"','"&amp;F36&amp;"','"&amp;G36&amp;"','"&amp;H36&amp;"','"&amp;I36&amp;"','"&amp;J36&amp;"','"&amp;K36&amp;"');"</f>
-        <v>('INDO_CMS_TEMPLATE_HEADER','TEMPLATE CODE','template_code','template_code','STRING','2','0','1','1','1');</v>
+        <v>('INDO_CMS_TEMPLATE_HEADER','ROW ID','row_id','row_id','INTEGER','1','1','1','0','0');</v>
       </c>
       <c r="N36" s="0" t="str">
         <f aca="false">"INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES"</f>
@@ -1895,27 +1901,27 @@
       </c>
       <c r="P36" s="0" t="str">
         <f aca="false">N36&amp;M36</f>
-        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_TEMPLATE_HEADER','TEMPLATE CODE','template_code','template_code','STRING','2','0','1','1','1');</v>
+        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_TEMPLATE_HEADER','ROW ID','row_id','row_id','INTEGER','1','1','1','0','0');</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>65</v>
+        <v>1</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>65</v>
+        <v>1</v>
       </c>
       <c r="F37" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G37" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H37" s="0" t="n">
         <v>0</v>
@@ -1931,7 +1937,7 @@
       </c>
       <c r="M37" s="0" t="str">
         <f aca="false">"('"&amp;B37&amp;"','"&amp;C37&amp;"','"&amp;D37&amp;"','"&amp;E37&amp;"','"&amp;F37&amp;"','"&amp;G37&amp;"','"&amp;H37&amp;"','"&amp;I37&amp;"','"&amp;J37&amp;"','"&amp;K37&amp;"');"</f>
-        <v>('INDO_CMS_TEMPLATE_HEADER','DATABASE NAME','database_name','database_name','STRING','3','0','1','1','1');</v>
+        <v>('INDO_CMS_TEMPLATE_HEADER','TEMPLATE CODE','template_code','template_code','STRING','2','0','1','1','1');</v>
       </c>
       <c r="N37" s="0" t="str">
         <f aca="false">"INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES"</f>
@@ -1939,12 +1945,12 @@
       </c>
       <c r="P37" s="0" t="str">
         <f aca="false">N37&amp;M37</f>
-        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_TEMPLATE_HEADER','DATABASE NAME','database_name','database_name','STRING','3','0','1','1','1');</v>
+        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_TEMPLATE_HEADER','TEMPLATE CODE','template_code','template_code','STRING','2','0','1','1','1');</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C38" s="0" t="s">
         <v>66</v>
@@ -1959,7 +1965,7 @@
         <v>16</v>
       </c>
       <c r="G38" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H38" s="0" t="n">
         <v>0</v>
@@ -1975,7 +1981,7 @@
       </c>
       <c r="M38" s="0" t="str">
         <f aca="false">"('"&amp;B38&amp;"','"&amp;C38&amp;"','"&amp;D38&amp;"','"&amp;E38&amp;"','"&amp;F38&amp;"','"&amp;G38&amp;"','"&amp;H38&amp;"','"&amp;I38&amp;"','"&amp;J38&amp;"','"&amp;K38&amp;"');"</f>
-        <v>('INDO_CMS_TEMPLATE_HEADER','DATABASE TABLE DELIMITER','database_table_delimiter','database_table_delimiter','STRING','4','0','1','1','1');</v>
+        <v>('INDO_CMS_TEMPLATE_HEADER','DATABASE NAME','database_name','database_name','STRING','3','0','1','1','1');</v>
       </c>
       <c r="N38" s="0" t="str">
         <f aca="false">"INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES"</f>
@@ -1983,12 +1989,12 @@
       </c>
       <c r="P38" s="0" t="str">
         <f aca="false">N38&amp;M38</f>
-        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_TEMPLATE_HEADER','DATABASE TABLE DELIMITER','database_table_delimiter','database_table_delimiter','STRING','4','0','1','1','1');</v>
+        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_TEMPLATE_HEADER','DATABASE NAME','database_name','database_name','STRING','3','0','1','1','1');</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C39" s="0" t="s">
         <v>68</v>
@@ -2003,7 +2009,7 @@
         <v>16</v>
       </c>
       <c r="G39" s="0" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H39" s="0" t="n">
         <v>0</v>
@@ -2019,7 +2025,7 @@
       </c>
       <c r="M39" s="0" t="str">
         <f aca="false">"('"&amp;B39&amp;"','"&amp;C39&amp;"','"&amp;D39&amp;"','"&amp;E39&amp;"','"&amp;F39&amp;"','"&amp;G39&amp;"','"&amp;H39&amp;"','"&amp;I39&amp;"','"&amp;J39&amp;"','"&amp;K39&amp;"');"</f>
-        <v>('INDO_CMS_TEMPLATE_HEADER','TABLE NAME','table_name','table_name','STRING','5','0','1','1','1');</v>
+        <v>('INDO_CMS_TEMPLATE_HEADER','DATABASE TABLE DELIMITER','database_table_delimiter','database_table_delimiter','STRING','4','0','1','1','1');</v>
       </c>
       <c r="N39" s="0" t="str">
         <f aca="false">"INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES"</f>
@@ -2027,12 +2033,12 @@
       </c>
       <c r="P39" s="0" t="str">
         <f aca="false">N39&amp;M39</f>
-        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_TEMPLATE_HEADER','TABLE NAME','table_name','table_name','STRING','5','0','1','1','1');</v>
+        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_TEMPLATE_HEADER','DATABASE TABLE DELIMITER','database_table_delimiter','database_table_delimiter','STRING','4','0','1','1','1');</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C40" s="0" t="s">
         <v>70</v>
@@ -2047,7 +2053,7 @@
         <v>16</v>
       </c>
       <c r="G40" s="0" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H40" s="0" t="n">
         <v>0</v>
@@ -2063,7 +2069,7 @@
       </c>
       <c r="M40" s="0" t="str">
         <f aca="false">"('"&amp;B40&amp;"','"&amp;C40&amp;"','"&amp;D40&amp;"','"&amp;E40&amp;"','"&amp;F40&amp;"','"&amp;G40&amp;"','"&amp;H40&amp;"','"&amp;I40&amp;"','"&amp;J40&amp;"','"&amp;K40&amp;"');"</f>
-        <v>('INDO_CMS_TEMPLATE_HEADER','DATABASE SERVICE','database_service','database_service','STRING','6','0','1','1','1');</v>
+        <v>('INDO_CMS_TEMPLATE_HEADER','TABLE NAME','table_name','table_name','STRING','5','0','1','1','1');</v>
       </c>
       <c r="N40" s="0" t="str">
         <f aca="false">"INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES"</f>
@@ -2071,12 +2077,12 @@
       </c>
       <c r="P40" s="0" t="str">
         <f aca="false">N40&amp;M40</f>
-        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_TEMPLATE_HEADER','DATABASE SERVICE','database_service','database_service','STRING','6','0','1','1','1');</v>
+        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_TEMPLATE_HEADER','TABLE NAME','table_name','table_name','STRING','5','0','1','1','1');</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C41" s="0" t="s">
         <v>72</v>
@@ -2091,7 +2097,7 @@
         <v>16</v>
       </c>
       <c r="G41" s="0" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H41" s="0" t="n">
         <v>0</v>
@@ -2107,7 +2113,7 @@
       </c>
       <c r="M41" s="0" t="str">
         <f aca="false">"('"&amp;B41&amp;"','"&amp;C41&amp;"','"&amp;D41&amp;"','"&amp;E41&amp;"','"&amp;F41&amp;"','"&amp;G41&amp;"','"&amp;H41&amp;"','"&amp;I41&amp;"','"&amp;J41&amp;"','"&amp;K41&amp;"');"</f>
-        <v>('INDO_CMS_TEMPLATE_HEADER','DATABASE CLASSNAME','database_classname','database_classname','STRING','7','0','1','1','1');</v>
+        <v>('INDO_CMS_TEMPLATE_HEADER','DATABASE SERVICE','database_service','database_service','STRING','6','0','1','1','1');</v>
       </c>
       <c r="N41" s="0" t="str">
         <f aca="false">"INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES"</f>
@@ -2115,12 +2121,12 @@
       </c>
       <c r="P41" s="0" t="str">
         <f aca="false">N41&amp;M41</f>
-        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_TEMPLATE_HEADER','DATABASE CLASSNAME','database_classname','database_classname','STRING','7','0','1','1','1');</v>
+        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_TEMPLATE_HEADER','DATABASE SERVICE','database_service','database_service','STRING','6','0','1','1','1');</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C42" s="0" t="s">
         <v>74</v>
@@ -2135,7 +2141,7 @@
         <v>16</v>
       </c>
       <c r="G42" s="0" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H42" s="0" t="n">
         <v>0</v>
@@ -2151,7 +2157,7 @@
       </c>
       <c r="M42" s="0" t="str">
         <f aca="false">"('"&amp;B42&amp;"','"&amp;C42&amp;"','"&amp;D42&amp;"','"&amp;E42&amp;"','"&amp;F42&amp;"','"&amp;G42&amp;"','"&amp;H42&amp;"','"&amp;I42&amp;"','"&amp;J42&amp;"','"&amp;K42&amp;"');"</f>
-        <v>('INDO_CMS_TEMPLATE_HEADER','DATABASE CONNECTION STRING','database_connection_string','database_connection_string','STRING','8','0','1','1','1');</v>
+        <v>('INDO_CMS_TEMPLATE_HEADER','DATABASE CLASSNAME','database_classname','database_classname','STRING','7','0','1','1','1');</v>
       </c>
       <c r="N42" s="0" t="str">
         <f aca="false">"INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES"</f>
@@ -2159,12 +2165,12 @@
       </c>
       <c r="P42" s="0" t="str">
         <f aca="false">N42&amp;M42</f>
-        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_TEMPLATE_HEADER','DATABASE CONNECTION STRING','database_connection_string','database_connection_string','STRING','8','0','1','1','1');</v>
+        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_TEMPLATE_HEADER','DATABASE CLASSNAME','database_classname','database_classname','STRING','7','0','1','1','1');</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C43" s="0" t="s">
         <v>76</v>
@@ -2179,7 +2185,7 @@
         <v>16</v>
       </c>
       <c r="G43" s="0" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H43" s="0" t="n">
         <v>0</v>
@@ -2195,7 +2201,7 @@
       </c>
       <c r="M43" s="0" t="str">
         <f aca="false">"('"&amp;B43&amp;"','"&amp;C43&amp;"','"&amp;D43&amp;"','"&amp;E43&amp;"','"&amp;F43&amp;"','"&amp;G43&amp;"','"&amp;H43&amp;"','"&amp;I43&amp;"','"&amp;J43&amp;"','"&amp;K43&amp;"');"</f>
-        <v>('INDO_CMS_TEMPLATE_HEADER','DATABASE USERNAME','database_username','database_username','STRING','9','0','1','1','1');</v>
+        <v>('INDO_CMS_TEMPLATE_HEADER','DATABASE CONNECTION STRING','database_connection_string','database_connection_string','STRING','8','0','1','1','1');</v>
       </c>
       <c r="N43" s="0" t="str">
         <f aca="false">"INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES"</f>
@@ -2203,12 +2209,12 @@
       </c>
       <c r="P43" s="0" t="str">
         <f aca="false">N43&amp;M43</f>
-        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_TEMPLATE_HEADER','DATABASE USERNAME','database_username','database_username','STRING','9','0','1','1','1');</v>
+        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_TEMPLATE_HEADER','DATABASE CONNECTION STRING','database_connection_string','database_connection_string','STRING','8','0','1','1','1');</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C44" s="0" t="s">
         <v>78</v>
@@ -2223,7 +2229,7 @@
         <v>16</v>
       </c>
       <c r="G44" s="0" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H44" s="0" t="n">
         <v>0</v>
@@ -2239,7 +2245,7 @@
       </c>
       <c r="M44" s="0" t="str">
         <f aca="false">"('"&amp;B44&amp;"','"&amp;C44&amp;"','"&amp;D44&amp;"','"&amp;E44&amp;"','"&amp;F44&amp;"','"&amp;G44&amp;"','"&amp;H44&amp;"','"&amp;I44&amp;"','"&amp;J44&amp;"','"&amp;K44&amp;"');"</f>
-        <v>('INDO_CMS_TEMPLATE_HEADER','DATABASE PASSWORD','database_password','database_password','STRING','10','0','1','1','1');</v>
+        <v>('INDO_CMS_TEMPLATE_HEADER','DATABASE USERNAME','database_username','database_username','STRING','9','0','1','1','1');</v>
       </c>
       <c r="N44" s="0" t="str">
         <f aca="false">"INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES"</f>
@@ -2247,87 +2253,87 @@
       </c>
       <c r="P44" s="0" t="str">
         <f aca="false">N44&amp;M44</f>
+        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_TEMPLATE_HEADER','DATABASE USERNAME','database_username','database_username','STRING','9','0','1','1','1');</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="E45" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="F45" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G45" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="H45" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I45" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J45" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K45" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M45" s="0" t="str">
+        <f aca="false">"('"&amp;B45&amp;"','"&amp;C45&amp;"','"&amp;D45&amp;"','"&amp;E45&amp;"','"&amp;F45&amp;"','"&amp;G45&amp;"','"&amp;H45&amp;"','"&amp;I45&amp;"','"&amp;J45&amp;"','"&amp;K45&amp;"');"</f>
+        <v>('INDO_CMS_TEMPLATE_HEADER','DATABASE PASSWORD','database_password','database_password','STRING','10','0','1','1','1');</v>
+      </c>
+      <c r="N45" s="0" t="str">
+        <f aca="false">"INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES"</f>
+        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES</v>
+      </c>
+      <c r="P45" s="0" t="str">
+        <f aca="false">N45&amp;M45</f>
         <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_TEMPLATE_HEADER','DATABASE PASSWORD','database_password','database_password','STRING','10','0','1','1','1');</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="C46" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D46" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="E46" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="F46" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G46" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H46" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I46" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J46" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K46" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M46" s="0" t="str">
-        <f aca="false">"('"&amp;B46&amp;"','"&amp;C46&amp;"','"&amp;D46&amp;"','"&amp;E46&amp;"','"&amp;F46&amp;"','"&amp;G46&amp;"','"&amp;H46&amp;"','"&amp;I46&amp;"','"&amp;J46&amp;"','"&amp;K46&amp;"');"</f>
-        <v>('INDO_CMS_TEMPLATE_DETAIL','ROW ID','row_id','row_id','INTEGER','1','1','1','0','0');</v>
-      </c>
-      <c r="N46" s="0" t="str">
-        <f aca="false">"INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES"</f>
-        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES</v>
-      </c>
-      <c r="P46" s="0" t="str">
-        <f aca="false">N46&amp;M46</f>
-        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_TEMPLATE_DETAIL','ROW ID','row_id','row_id','INTEGER','1','1','1','0','0');</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>63</v>
+        <v>12</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G47" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H47" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I47" s="0" t="n">
         <v>1</v>
       </c>
       <c r="J47" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K47" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M47" s="0" t="str">
         <f aca="false">"('"&amp;B47&amp;"','"&amp;C47&amp;"','"&amp;D47&amp;"','"&amp;E47&amp;"','"&amp;F47&amp;"','"&amp;G47&amp;"','"&amp;H47&amp;"','"&amp;I47&amp;"','"&amp;J47&amp;"','"&amp;K47&amp;"');"</f>
-        <v>('INDO_CMS_TEMPLATE_DETAIL','TEMPLATE CODE','template_code','template_code','STRING','2','0','1','1','1');</v>
+        <v>('INDO_CMS_TEMPLATE_DETAIL','ROW ID','row_id','row_id','INTEGER','1','1','1','0','0');</v>
       </c>
       <c r="N47" s="0" t="str">
         <f aca="false">"INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES"</f>
@@ -2335,27 +2341,27 @@
       </c>
       <c r="P47" s="0" t="str">
         <f aca="false">N47&amp;M47</f>
-        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_TEMPLATE_DETAIL','TEMPLATE CODE','template_code','template_code','STRING','2','0','1','1','1');</v>
+        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_TEMPLATE_DETAIL','ROW ID','row_id','row_id','INTEGER','1','1','1','0','0');</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="D48" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E48" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="F48" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G48" s="0" t="n">
         <v>2</v>
-      </c>
-      <c r="E48" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="F48" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G48" s="0" t="n">
-        <v>3</v>
       </c>
       <c r="H48" s="0" t="n">
         <v>0</v>
@@ -2371,7 +2377,7 @@
       </c>
       <c r="M48" s="0" t="str">
         <f aca="false">"('"&amp;B48&amp;"','"&amp;C48&amp;"','"&amp;D48&amp;"','"&amp;E48&amp;"','"&amp;F48&amp;"','"&amp;G48&amp;"','"&amp;H48&amp;"','"&amp;I48&amp;"','"&amp;J48&amp;"','"&amp;K48&amp;"');"</f>
-        <v>('INDO_CMS_TEMPLATE_DETAIL','WEB COLUMN','web_column','web_column','STRING','3','0','1','1','1');</v>
+        <v>('INDO_CMS_TEMPLATE_DETAIL','TEMPLATE CODE','template_code','template_code','STRING','2','0','1','1','1');</v>
       </c>
       <c r="N48" s="0" t="str">
         <f aca="false">"INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES"</f>
@@ -2379,27 +2385,27 @@
       </c>
       <c r="P48" s="0" t="str">
         <f aca="false">N48&amp;M48</f>
-        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_TEMPLATE_DETAIL','WEB COLUMN','web_column','web_column','STRING','3','0','1','1','1');</v>
+        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_TEMPLATE_DETAIL','TEMPLATE CODE','template_code','template_code','STRING','2','0','1','1','1');</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D49" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E49" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="F49" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G49" s="0" t="n">
         <v>3</v>
-      </c>
-      <c r="E49" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="F49" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G49" s="0" t="n">
-        <v>4</v>
       </c>
       <c r="H49" s="0" t="n">
         <v>0</v>
@@ -2415,7 +2421,7 @@
       </c>
       <c r="M49" s="0" t="str">
         <f aca="false">"('"&amp;B49&amp;"','"&amp;C49&amp;"','"&amp;D49&amp;"','"&amp;E49&amp;"','"&amp;F49&amp;"','"&amp;G49&amp;"','"&amp;H49&amp;"','"&amp;I49&amp;"','"&amp;J49&amp;"','"&amp;K49&amp;"');"</f>
-        <v>('INDO_CMS_TEMPLATE_DETAIL','DATABASE COLUMN','database_column','database_column','STRING','4','0','1','1','1');</v>
+        <v>('INDO_CMS_TEMPLATE_DETAIL','WEB COLUMN','web_column','web_column','STRING','3','0','1','1','1');</v>
       </c>
       <c r="N49" s="0" t="str">
         <f aca="false">"INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES"</f>
@@ -2423,27 +2429,27 @@
       </c>
       <c r="P49" s="0" t="str">
         <f aca="false">N49&amp;M49</f>
-        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_TEMPLATE_DETAIL','DATABASE COLUMN','database_column','database_column','STRING','4','0','1','1','1');</v>
+        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_TEMPLATE_DETAIL','WEB COLUMN','web_column','web_column','STRING','3','0','1','1','1');</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D50" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E50" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="F50" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G50" s="0" t="n">
         <v>4</v>
-      </c>
-      <c r="E50" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="F50" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G50" s="0" t="n">
-        <v>5</v>
       </c>
       <c r="H50" s="0" t="n">
         <v>0</v>
@@ -2459,7 +2465,7 @@
       </c>
       <c r="M50" s="0" t="str">
         <f aca="false">"('"&amp;B50&amp;"','"&amp;C50&amp;"','"&amp;D50&amp;"','"&amp;E50&amp;"','"&amp;F50&amp;"','"&amp;G50&amp;"','"&amp;H50&amp;"','"&amp;I50&amp;"','"&amp;J50&amp;"','"&amp;K50&amp;"');"</f>
-        <v>('INDO_CMS_TEMPLATE_DETAIL','QUERY COLUMN','query_column','query_column','STRING','5','0','1','1','1');</v>
+        <v>('INDO_CMS_TEMPLATE_DETAIL','DATABASE COLUMN','database_column','database_column','STRING','4','0','1','1','1');</v>
       </c>
       <c r="N50" s="0" t="str">
         <f aca="false">"INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES"</f>
@@ -2467,27 +2473,27 @@
       </c>
       <c r="P50" s="0" t="str">
         <f aca="false">N50&amp;M50</f>
-        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_TEMPLATE_DETAIL','QUERY COLUMN','query_column','query_column','STRING','5','0','1','1','1');</v>
+        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_TEMPLATE_DETAIL','DATABASE COLUMN','database_column','database_column','STRING','4','0','1','1','1');</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D51" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E51" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F51" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G51" s="0" t="n">
         <v>5</v>
-      </c>
-      <c r="E51" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="F51" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G51" s="0" t="n">
-        <v>6</v>
       </c>
       <c r="H51" s="0" t="n">
         <v>0</v>
@@ -2503,7 +2509,7 @@
       </c>
       <c r="M51" s="0" t="str">
         <f aca="false">"('"&amp;B51&amp;"','"&amp;C51&amp;"','"&amp;D51&amp;"','"&amp;E51&amp;"','"&amp;F51&amp;"','"&amp;G51&amp;"','"&amp;H51&amp;"','"&amp;I51&amp;"','"&amp;J51&amp;"','"&amp;K51&amp;"');"</f>
-        <v>('INDO_CMS_TEMPLATE_DETAIL','DATA TYPE','data_type','data_type','STRING','6','0','1','1','1');</v>
+        <v>('INDO_CMS_TEMPLATE_DETAIL','QUERY COLUMN','query_column','query_column','STRING','5','0','1','1','1');</v>
       </c>
       <c r="N51" s="0" t="str">
         <f aca="false">"INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES"</f>
@@ -2511,27 +2517,27 @@
       </c>
       <c r="P51" s="0" t="str">
         <f aca="false">N51&amp;M51</f>
-        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_TEMPLATE_DETAIL','DATA TYPE','data_type','data_type','STRING','6','0','1','1','1');</v>
+        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_TEMPLATE_DETAIL','QUERY COLUMN','query_column','query_column','STRING','5','0','1','1','1');</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D52" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="E52" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="F52" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G52" s="0" t="n">
         <v>6</v>
-      </c>
-      <c r="E52" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="F52" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G52" s="0" t="n">
-        <v>7</v>
       </c>
       <c r="H52" s="0" t="n">
         <v>0</v>
@@ -2547,7 +2553,7 @@
       </c>
       <c r="M52" s="0" t="str">
         <f aca="false">"('"&amp;B52&amp;"','"&amp;C52&amp;"','"&amp;D52&amp;"','"&amp;E52&amp;"','"&amp;F52&amp;"','"&amp;G52&amp;"','"&amp;H52&amp;"','"&amp;I52&amp;"','"&amp;J52&amp;"','"&amp;K52&amp;"');"</f>
-        <v>('INDO_CMS_TEMPLATE_DETAIL','SEQUENCE','sequence','sequence','INTEGER','7','0','1','1','1');</v>
+        <v>('INDO_CMS_TEMPLATE_DETAIL','DATA TYPE','data_type','data_type','STRING','6','0','1','1','1');</v>
       </c>
       <c r="N52" s="0" t="str">
         <f aca="false">"INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES"</f>
@@ -2555,27 +2561,27 @@
       </c>
       <c r="P52" s="0" t="str">
         <f aca="false">N52&amp;M52</f>
-        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_TEMPLATE_DETAIL','SEQUENCE','sequence','sequence','INTEGER','7','0','1','1','1');</v>
+        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_TEMPLATE_DETAIL','DATA TYPE','data_type','data_type','STRING','6','0','1','1','1');</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D53" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E53" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="F53" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G53" s="0" t="n">
         <v>7</v>
-      </c>
-      <c r="E53" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="F53" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G53" s="0" t="n">
-        <v>8</v>
       </c>
       <c r="H53" s="0" t="n">
         <v>0</v>
@@ -2591,7 +2597,7 @@
       </c>
       <c r="M53" s="0" t="str">
         <f aca="false">"('"&amp;B53&amp;"','"&amp;C53&amp;"','"&amp;D53&amp;"','"&amp;E53&amp;"','"&amp;F53&amp;"','"&amp;G53&amp;"','"&amp;H53&amp;"','"&amp;I53&amp;"','"&amp;J53&amp;"','"&amp;K53&amp;"');"</f>
-        <v>('INDO_CMS_TEMPLATE_DETAIL','IS PRIMARY','is_primary','is_primary','STRING','8','0','1','1','1');</v>
+        <v>('INDO_CMS_TEMPLATE_DETAIL','SEQUENCE','sequence','sequence','INTEGER','7','0','1','1','1');</v>
       </c>
       <c r="N53" s="0" t="str">
         <f aca="false">"INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES"</f>
@@ -2599,27 +2605,27 @@
       </c>
       <c r="P53" s="0" t="str">
         <f aca="false">N53&amp;M53</f>
-        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_TEMPLATE_DETAIL','IS PRIMARY','is_primary','is_primary','STRING','8','0','1','1','1');</v>
+        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_TEMPLATE_DETAIL','SEQUENCE','sequence','sequence','INTEGER','7','0','1','1','1');</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D54" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E54" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="F54" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G54" s="0" t="n">
         <v>8</v>
-      </c>
-      <c r="E54" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F54" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G54" s="0" t="n">
-        <v>9</v>
       </c>
       <c r="H54" s="0" t="n">
         <v>0</v>
@@ -2635,7 +2641,7 @@
       </c>
       <c r="M54" s="0" t="str">
         <f aca="false">"('"&amp;B54&amp;"','"&amp;C54&amp;"','"&amp;D54&amp;"','"&amp;E54&amp;"','"&amp;F54&amp;"','"&amp;G54&amp;"','"&amp;H54&amp;"','"&amp;I54&amp;"','"&amp;J54&amp;"','"&amp;K54&amp;"');"</f>
-        <v>('INDO_CMS_TEMPLATE_DETAIL','IS SHOW','is_show','is_show','STRING','9','0','1','1','1');</v>
+        <v>('INDO_CMS_TEMPLATE_DETAIL','IS PRIMARY','is_primary','is_primary','STRING','8','0','1','1','1');</v>
       </c>
       <c r="N54" s="0" t="str">
         <f aca="false">"INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES"</f>
@@ -2643,27 +2649,27 @@
       </c>
       <c r="P54" s="0" t="str">
         <f aca="false">N54&amp;M54</f>
-        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_TEMPLATE_DETAIL','IS SHOW','is_show','is_show','STRING','9','0','1','1','1');</v>
+        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_TEMPLATE_DETAIL','IS PRIMARY','is_primary','is_primary','STRING','8','0','1','1','1');</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D55" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E55" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F55" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G55" s="0" t="n">
         <v>9</v>
-      </c>
-      <c r="E55" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F55" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G55" s="0" t="n">
-        <v>10</v>
       </c>
       <c r="H55" s="0" t="n">
         <v>0</v>
@@ -2679,7 +2685,7 @@
       </c>
       <c r="M55" s="0" t="str">
         <f aca="false">"('"&amp;B55&amp;"','"&amp;C55&amp;"','"&amp;D55&amp;"','"&amp;E55&amp;"','"&amp;F55&amp;"','"&amp;G55&amp;"','"&amp;H55&amp;"','"&amp;I55&amp;"','"&amp;J55&amp;"','"&amp;K55&amp;"');"</f>
-        <v>('INDO_CMS_TEMPLATE_DETAIL','IS CREATE','is_create','is_create','STRING','10','0','1','1','1');</v>
+        <v>('INDO_CMS_TEMPLATE_DETAIL','IS SHOW','is_show','is_show','STRING','9','0','1','1','1');</v>
       </c>
       <c r="N55" s="0" t="str">
         <f aca="false">"INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES"</f>
@@ -2687,27 +2693,27 @@
       </c>
       <c r="P55" s="0" t="str">
         <f aca="false">N55&amp;M55</f>
-        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_TEMPLATE_DETAIL','IS CREATE','is_create','is_create','STRING','10','0','1','1','1');</v>
+        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_TEMPLATE_DETAIL','IS SHOW','is_show','is_show','STRING','9','0','1','1','1');</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D56" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E56" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F56" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G56" s="0" t="n">
         <v>10</v>
-      </c>
-      <c r="E56" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F56" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G56" s="0" t="n">
-        <v>11</v>
       </c>
       <c r="H56" s="0" t="n">
         <v>0</v>
@@ -2723,7 +2729,7 @@
       </c>
       <c r="M56" s="0" t="str">
         <f aca="false">"('"&amp;B56&amp;"','"&amp;C56&amp;"','"&amp;D56&amp;"','"&amp;E56&amp;"','"&amp;F56&amp;"','"&amp;G56&amp;"','"&amp;H56&amp;"','"&amp;I56&amp;"','"&amp;J56&amp;"','"&amp;K56&amp;"');"</f>
-        <v>('INDO_CMS_TEMPLATE_DETAIL','IS EDIT','is_edit','is_edit','STRING','11','0','1','1','1');</v>
+        <v>('INDO_CMS_TEMPLATE_DETAIL','IS CREATE','is_create','is_create','STRING','10','0','1','1','1');</v>
       </c>
       <c r="N56" s="0" t="str">
         <f aca="false">"INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES"</f>
@@ -2731,27 +2737,27 @@
       </c>
       <c r="P56" s="0" t="str">
         <f aca="false">N56&amp;M56</f>
-        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_TEMPLATE_DETAIL','IS EDIT','is_edit','is_edit','STRING','11','0','1','1','1');</v>
+        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_TEMPLATE_DETAIL','IS CREATE','is_create','is_create','STRING','10','0','1','1','1');</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>91</v>
+        <v>10</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>91</v>
+        <v>10</v>
       </c>
       <c r="F57" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G57" s="0" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H57" s="0" t="n">
         <v>0</v>
@@ -2767,7 +2773,7 @@
       </c>
       <c r="M57" s="0" t="str">
         <f aca="false">"('"&amp;B57&amp;"','"&amp;C57&amp;"','"&amp;D57&amp;"','"&amp;E57&amp;"','"&amp;F57&amp;"','"&amp;G57&amp;"','"&amp;H57&amp;"','"&amp;I57&amp;"','"&amp;J57&amp;"','"&amp;K57&amp;"');"</f>
-        <v>('INDO_CMS_TEMPLATE_DETAIL','LOOKUP QUERY','lookup_query','lookup_query','STRING','12','0','1','1','1');</v>
+        <v>('INDO_CMS_TEMPLATE_DETAIL','IS EDIT','is_edit','is_edit','STRING','11','0','1','1','1');</v>
       </c>
       <c r="N57" s="0" t="str">
         <f aca="false">"INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES"</f>
@@ -2775,6 +2781,50 @@
       </c>
       <c r="P57" s="0" t="str">
         <f aca="false">N57&amp;M57</f>
+        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_TEMPLATE_DETAIL','IS EDIT','is_edit','is_edit','STRING','11','0','1','1','1');</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B58" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C58" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="D58" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E58" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="F58" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G58" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="H58" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I58" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J58" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K58" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M58" s="0" t="str">
+        <f aca="false">"('"&amp;B58&amp;"','"&amp;C58&amp;"','"&amp;D58&amp;"','"&amp;E58&amp;"','"&amp;F58&amp;"','"&amp;G58&amp;"','"&amp;H58&amp;"','"&amp;I58&amp;"','"&amp;J58&amp;"','"&amp;K58&amp;"');"</f>
+        <v>('INDO_CMS_TEMPLATE_DETAIL','LOOKUP QUERY','lookup_query','lookup_query','STRING','12','0','1','1','1');</v>
+      </c>
+      <c r="N58" s="0" t="str">
+        <f aca="false">"INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES"</f>
+        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES</v>
+      </c>
+      <c r="P58" s="0" t="str">
+        <f aca="false">N58&amp;M58</f>
         <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_TEMPLATE_DETAIL','LOOKUP QUERY','lookup_query','lookup_query','STRING','12','0','1','1','1');</v>
       </c>
     </row>
@@ -2797,7 +2847,7 @@
   <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="P26:P34 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2852,7 +2902,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>12</v>
@@ -2896,16 +2946,16 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>16</v>
@@ -2940,16 +2990,16 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>16</v>
@@ -2984,16 +3034,16 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>16</v>
@@ -3028,7 +3078,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>12</v>
@@ -3072,16 +3122,16 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>16</v>
@@ -3116,16 +3166,16 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F9" s="0" t="s">
         <v>16</v>
@@ -3160,16 +3210,16 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F10" s="0" t="s">
         <v>16</v>
@@ -3204,16 +3254,16 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="F11" s="0" t="s">
         <v>16</v>
@@ -3248,16 +3298,16 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F12" s="0" t="s">
         <v>16</v>
@@ -3292,16 +3342,16 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="F13" s="0" t="s">
         <v>16</v>
@@ -3336,7 +3386,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>12</v>
@@ -3380,16 +3430,16 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F16" s="0" t="s">
         <v>16</v>
@@ -3424,16 +3474,16 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F17" s="0" t="s">
         <v>16</v>
@@ -3468,16 +3518,16 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="F18" s="0" t="s">
         <v>16</v>
@@ -3512,16 +3562,16 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="F19" s="0" t="s">
         <v>16</v>
@@ -3556,19 +3606,19 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="G20" s="0" t="n">
         <v>6</v>
@@ -3600,19 +3650,19 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D21" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="F21" s="0" t="s">
         <v>119</v>
-      </c>
-      <c r="E21" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="F21" s="0" t="s">
-        <v>117</v>
       </c>
       <c r="G21" s="0" t="n">
         <v>7</v>
@@ -3645,7 +3695,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
final integration with single approver
</commit_message>
<xml_diff>
--- a/sql/INDO_CMS_TEMPLATE_QUERY.xlsx
+++ b/sql/INDO_CMS_TEMPLATE_QUERY.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="159">
   <si>
     <t xml:space="preserve">row_id</t>
   </si>
@@ -312,6 +312,12 @@
     <t xml:space="preserve">lookup_query</t>
   </si>
   <si>
+    <t xml:space="preserve">MAX LENGTH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max_length</t>
+  </si>
+  <si>
     <t xml:space="preserve">INDO_CMS_USER_APPROVER</t>
   </si>
   <si>
@@ -331,6 +337,24 @@
   </si>
   <si>
     <t xml:space="preserve">approver_sequence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INDO_CMS_JOB_HEADER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JOB ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">job_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JOB DESCRIPTION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">job_description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INDO_CMS_JOB_DETAIL</t>
   </si>
   <si>
     <t xml:space="preserve">INDO_CMS_BANK</t>
@@ -575,10 +599,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P65"/>
+  <dimension ref="A1:P74"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P65" activeCellId="0" sqref="P61:P65"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A48" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C74" activeCellId="0" sqref="C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -587,7 +611,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.91"/>
@@ -2964,84 +2988,84 @@
         <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_TEMPLATE_DETAIL','LOOKUP QUERY','lookup_query','lookup_query','STRING','12','0','1','1','1');</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="0" t="s">
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B60" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="C60" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="C61" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D61" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="E61" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="F61" s="0" t="s">
+      <c r="D60" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="E60" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="F60" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="G61" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H61" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I61" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J61" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K61" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M61" s="0" t="str">
-        <f aca="false">"('"&amp;B61&amp;"','"&amp;C61&amp;"','"&amp;D61&amp;"','"&amp;E61&amp;"','"&amp;F61&amp;"','"&amp;G61&amp;"','"&amp;H61&amp;"','"&amp;I61&amp;"','"&amp;J61&amp;"','"&amp;K61&amp;"');"</f>
-        <v>('INDO_CMS_USER_APPROVER','ROW ID','row_id','row_id','INTEGER','1','1','1','0','0');</v>
-      </c>
-      <c r="N61" s="0" t="str">
-        <f aca="false">"INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES"</f>
-        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES</v>
-      </c>
-      <c r="P61" s="0" t="str">
-        <f aca="false">N61&amp;M61</f>
-        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_USER_APPROVER','ROW ID','row_id','row_id','INTEGER','1','1','1','0','0');</v>
+      <c r="G60" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="H60" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I60" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J60" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K60" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M60" s="0" t="str">
+        <f aca="false">"('"&amp;B60&amp;"','"&amp;C60&amp;"','"&amp;D60&amp;"','"&amp;E60&amp;"','"&amp;F60&amp;"','"&amp;G60&amp;"','"&amp;H60&amp;"','"&amp;I60&amp;"','"&amp;J60&amp;"','"&amp;K60&amp;"');"</f>
+        <v>('INDO_CMS_TEMPLATE_DETAIL','MAX LENGTH','max_length','max_length','INTEGER','13','0','1','1','1');</v>
+      </c>
+      <c r="N60" s="0" t="str">
+        <f aca="false">"INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES"</f>
+        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES</v>
+      </c>
+      <c r="P60" s="0" t="str">
+        <f aca="false">N60&amp;M60</f>
+        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_TEMPLATE_DETAIL','MAX LENGTH','max_length','max_length','INTEGER','13','0','1','1','1');</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="F62" s="0" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G62" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H62" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I62" s="0" t="n">
         <v>1</v>
       </c>
       <c r="J62" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K62" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M62" s="0" t="str">
         <f aca="false">"('"&amp;B62&amp;"','"&amp;C62&amp;"','"&amp;D62&amp;"','"&amp;E62&amp;"','"&amp;F62&amp;"','"&amp;G62&amp;"','"&amp;H62&amp;"','"&amp;I62&amp;"','"&amp;J62&amp;"','"&amp;K62&amp;"');"</f>
-        <v>('INDO_CMS_USER_APPROVER','USERNAME','username','username','STRING','2','0','1','1','1');</v>
+        <v>('INDO_CMS_USER_APPROVER','ROW ID','row_id','row_id','INTEGER','1','1','1','0','0');</v>
       </c>
       <c r="N62" s="0" t="str">
         <f aca="false">"INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES"</f>
@@ -3049,27 +3073,27 @@
       </c>
       <c r="P62" s="0" t="str">
         <f aca="false">N62&amp;M62</f>
-        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_USER_APPROVER','USERNAME','username','username','STRING','2','0','1','1','1');</v>
+        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_USER_APPROVER','ROW ID','row_id','row_id','INTEGER','1','1','1','0','0');</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>97</v>
+        <v>14</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>98</v>
+        <v>15</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>98</v>
+        <v>15</v>
       </c>
       <c r="F63" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G63" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H63" s="0" t="n">
         <v>0</v>
@@ -3085,7 +3109,7 @@
       </c>
       <c r="M63" s="0" t="str">
         <f aca="false">"('"&amp;B63&amp;"','"&amp;C63&amp;"','"&amp;D63&amp;"','"&amp;E63&amp;"','"&amp;F63&amp;"','"&amp;G63&amp;"','"&amp;H63&amp;"','"&amp;I63&amp;"','"&amp;J63&amp;"','"&amp;K63&amp;"');"</f>
-        <v>('INDO_CMS_USER_APPROVER','APPROVER USERNAME','approver_username','approver_username','STRING','3','0','1','1','1');</v>
+        <v>('INDO_CMS_USER_APPROVER','USERNAME','username','username','STRING','2','0','1','1','1');</v>
       </c>
       <c r="N63" s="0" t="str">
         <f aca="false">"INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES"</f>
@@ -3093,27 +3117,27 @@
       </c>
       <c r="P63" s="0" t="str">
         <f aca="false">N63&amp;M63</f>
-        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_USER_APPROVER','APPROVER USERNAME','approver_username','approver_username','STRING','3','0','1','1','1');</v>
+        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_USER_APPROVER','USERNAME','username','username','STRING','2','0','1','1','1');</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>99</v>
+        <v>27</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>100</v>
+        <v>28</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>100</v>
+        <v>28</v>
       </c>
       <c r="F64" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G64" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H64" s="0" t="n">
         <v>0</v>
@@ -3129,7 +3153,7 @@
       </c>
       <c r="M64" s="0" t="str">
         <f aca="false">"('"&amp;B64&amp;"','"&amp;C64&amp;"','"&amp;D64&amp;"','"&amp;E64&amp;"','"&amp;F64&amp;"','"&amp;G64&amp;"','"&amp;H64&amp;"','"&amp;I64&amp;"','"&amp;J64&amp;"','"&amp;K64&amp;"');"</f>
-        <v>('INDO_CMS_USER_APPROVER','APPROVER ROLE','approver_role','approver_role','STRING','4','0','1','1','1');</v>
+        <v>('INDO_CMS_USER_APPROVER','ROLE ID','role_id','role_id','STRING','3','0','1','1','1');</v>
       </c>
       <c r="N64" s="0" t="str">
         <f aca="false">"INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES"</f>
@@ -3137,27 +3161,27 @@
       </c>
       <c r="P64" s="0" t="str">
         <f aca="false">N64&amp;M64</f>
-        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_USER_APPROVER','APPROVER ROLE','approver_role','approver_role','STRING','4','0','1','1','1');</v>
+        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_USER_APPROVER','ROLE ID','role_id','role_id','STRING','3','0','1','1','1');</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F65" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G65" s="0" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H65" s="0" t="n">
         <v>0</v>
@@ -3173,7 +3197,7 @@
       </c>
       <c r="M65" s="0" t="str">
         <f aca="false">"('"&amp;B65&amp;"','"&amp;C65&amp;"','"&amp;D65&amp;"','"&amp;E65&amp;"','"&amp;F65&amp;"','"&amp;G65&amp;"','"&amp;H65&amp;"','"&amp;I65&amp;"','"&amp;J65&amp;"','"&amp;K65&amp;"');"</f>
-        <v>('INDO_CMS_USER_APPROVER','APPROVER SEQUENCE','approver_sequence','approver_sequence','STRING','5','0','1','1','1');</v>
+        <v>('INDO_CMS_USER_APPROVER','APPROVER USERNAME','approver_username','approver_username','STRING','4','0','1','1','1');</v>
       </c>
       <c r="N65" s="0" t="str">
         <f aca="false">"INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES"</f>
@@ -3181,7 +3205,315 @@
       </c>
       <c r="P65" s="0" t="str">
         <f aca="false">N65&amp;M65</f>
-        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_USER_APPROVER','APPROVER SEQUENCE','approver_sequence','approver_sequence','STRING','5','0','1','1','1');</v>
+        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_USER_APPROVER','APPROVER USERNAME','approver_username','approver_username','STRING','4','0','1','1','1');</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B66" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="C66" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="D66" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="E66" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="F66" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G66" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="H66" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I66" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J66" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K66" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M66" s="0" t="str">
+        <f aca="false">"('"&amp;B66&amp;"','"&amp;C66&amp;"','"&amp;D66&amp;"','"&amp;E66&amp;"','"&amp;F66&amp;"','"&amp;G66&amp;"','"&amp;H66&amp;"','"&amp;I66&amp;"','"&amp;J66&amp;"','"&amp;K66&amp;"');"</f>
+        <v>('INDO_CMS_USER_APPROVER','APPROVER ROLE','approver_role','approver_role','STRING','5','0','1','1','1');</v>
+      </c>
+      <c r="N66" s="0" t="str">
+        <f aca="false">"INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES"</f>
+        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES</v>
+      </c>
+      <c r="P66" s="0" t="str">
+        <f aca="false">N66&amp;M66</f>
+        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_USER_APPROVER','APPROVER ROLE','approver_role','approver_role','STRING','5','0','1','1','1');</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B67" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="C67" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="D67" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="E67" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="F67" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G67" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H67" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I67" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J67" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K67" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M67" s="0" t="str">
+        <f aca="false">"('"&amp;B67&amp;"','"&amp;C67&amp;"','"&amp;D67&amp;"','"&amp;E67&amp;"','"&amp;F67&amp;"','"&amp;G67&amp;"','"&amp;H67&amp;"','"&amp;I67&amp;"','"&amp;J67&amp;"','"&amp;K67&amp;"');"</f>
+        <v>('INDO_CMS_USER_APPROVER','APPROVER SEQUENCE','approver_sequence','approver_sequence','STRING','6','0','1','1','1');</v>
+      </c>
+      <c r="N67" s="0" t="str">
+        <f aca="false">"INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES"</f>
+        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES</v>
+      </c>
+      <c r="P67" s="0" t="str">
+        <f aca="false">N67&amp;M67</f>
+        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_USER_APPROVER','APPROVER SEQUENCE','approver_sequence','approver_sequence','STRING','6','0','1','1','1');</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B69" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="C69" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D69" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="E69" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="F69" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G69" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H69" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I69" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J69" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K69" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M69" s="0" t="str">
+        <f aca="false">"('"&amp;B69&amp;"','"&amp;C69&amp;"','"&amp;D69&amp;"','"&amp;E69&amp;"','"&amp;F69&amp;"','"&amp;G69&amp;"','"&amp;H69&amp;"','"&amp;I69&amp;"','"&amp;J69&amp;"','"&amp;K69&amp;"');"</f>
+        <v>('INDO_CMS_JOB_HEADER','ROW ID','row_id','row_id','INTEGER','1','1','1','0','0');</v>
+      </c>
+      <c r="N69" s="0" t="str">
+        <f aca="false">"INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES"</f>
+        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES</v>
+      </c>
+      <c r="P69" s="0" t="str">
+        <f aca="false">N69&amp;M69</f>
+        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_JOB_HEADER','ROW ID','row_id','row_id','INTEGER','1','1','1','0','0');</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B70" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="C70" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="D70" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="E70" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="F70" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G70" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H70" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I70" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J70" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K70" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M70" s="0" t="str">
+        <f aca="false">"('"&amp;B70&amp;"','"&amp;C70&amp;"','"&amp;D70&amp;"','"&amp;E70&amp;"','"&amp;F70&amp;"','"&amp;G70&amp;"','"&amp;H70&amp;"','"&amp;I70&amp;"','"&amp;J70&amp;"','"&amp;K70&amp;"');"</f>
+        <v>('INDO_CMS_JOB_HEADER','JOB ID','job_id','job_id','STRING','2','0','1','1','1');</v>
+      </c>
+      <c r="N70" s="0" t="str">
+        <f aca="false">"INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES"</f>
+        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES</v>
+      </c>
+      <c r="P70" s="0" t="str">
+        <f aca="false">N70&amp;M70</f>
+        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_JOB_HEADER','JOB ID','job_id','job_id','STRING','2','0','1','1','1');</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B71" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="C71" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="D71" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="E71" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="F71" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G71" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H71" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I71" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J71" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K71" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M71" s="0" t="str">
+        <f aca="false">"('"&amp;B71&amp;"','"&amp;C71&amp;"','"&amp;D71&amp;"','"&amp;E71&amp;"','"&amp;F71&amp;"','"&amp;G71&amp;"','"&amp;H71&amp;"','"&amp;I71&amp;"','"&amp;J71&amp;"','"&amp;K71&amp;"');"</f>
+        <v>('INDO_CMS_JOB_HEADER','JOB DESCRIPTION','job_description','job_description','STRING','3','0','1','1','1');</v>
+      </c>
+      <c r="N71" s="0" t="str">
+        <f aca="false">"INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES"</f>
+        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES</v>
+      </c>
+      <c r="P71" s="0" t="str">
+        <f aca="false">N71&amp;M71</f>
+        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_JOB_HEADER','JOB DESCRIPTION','job_description','job_description','STRING','3','0','1','1','1');</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B73" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="C73" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D73" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="E73" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="F73" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G73" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H73" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I73" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J73" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K73" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M73" s="0" t="str">
+        <f aca="false">"('"&amp;B73&amp;"','"&amp;C73&amp;"','"&amp;D73&amp;"','"&amp;E73&amp;"','"&amp;F73&amp;"','"&amp;G73&amp;"','"&amp;H73&amp;"','"&amp;I73&amp;"','"&amp;J73&amp;"','"&amp;K73&amp;"');"</f>
+        <v>('INDO_CMS_JOB_DETAIL','ROW ID','row_id','row_id','INTEGER','1','1','1','0','0');</v>
+      </c>
+      <c r="N73" s="0" t="str">
+        <f aca="false">"INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES"</f>
+        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES</v>
+      </c>
+      <c r="P73" s="0" t="str">
+        <f aca="false">N73&amp;M73</f>
+        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_JOB_DETAIL','ROW ID','row_id','row_id','INTEGER','1','1','1','0','0');</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B74" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="C74" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="D74" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="E74" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="F74" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G74" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H74" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I74" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J74" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K74" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M74" s="0" t="str">
+        <f aca="false">"('"&amp;B74&amp;"','"&amp;C74&amp;"','"&amp;D74&amp;"','"&amp;E74&amp;"','"&amp;F74&amp;"','"&amp;G74&amp;"','"&amp;H74&amp;"','"&amp;I74&amp;"','"&amp;J74&amp;"','"&amp;K74&amp;"');"</f>
+        <v>('INDO_CMS_JOB_DETAIL','JOB ID','job_id','job_id','STRING','2','0','1','1','1');</v>
+      </c>
+      <c r="N74" s="0" t="str">
+        <f aca="false">"INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES"</f>
+        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES</v>
+      </c>
+      <c r="P74" s="0" t="str">
+        <f aca="false">N74&amp;M74</f>
+        <v>INSERT INTO INDO_CMS_TEMPLATE_DETAIL (template_code,web_column,database_column,query_column,data_type,sequence,is_primary,is_show,is_create,is_edit) VALUES('INDO_CMS_JOB_DETAIL','JOB ID','job_id','job_id','STRING','2','0','1','1','1');</v>
       </c>
     </row>
   </sheetData>
@@ -3203,7 +3535,7 @@
   <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="P61:P65 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3258,7 +3590,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>12</v>
@@ -3302,16 +3634,16 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>16</v>
@@ -3346,16 +3678,16 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>16</v>
@@ -3390,16 +3722,16 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>16</v>
@@ -3434,7 +3766,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>12</v>
@@ -3478,16 +3810,16 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>16</v>
@@ -3522,16 +3854,16 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="F9" s="0" t="s">
         <v>16</v>
@@ -3566,16 +3898,16 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="F10" s="0" t="s">
         <v>16</v>
@@ -3610,16 +3942,16 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="F11" s="0" t="s">
         <v>16</v>
@@ -3654,16 +3986,16 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="F12" s="0" t="s">
         <v>16</v>
@@ -3698,16 +4030,16 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="F13" s="0" t="s">
         <v>16</v>
@@ -3742,7 +4074,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>12</v>
@@ -3786,16 +4118,16 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="F16" s="0" t="s">
         <v>16</v>
@@ -3830,16 +4162,16 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="F17" s="0" t="s">
         <v>16</v>
@@ -3874,16 +4206,16 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="F18" s="0" t="s">
         <v>16</v>
@@ -3918,16 +4250,16 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="F19" s="0" t="s">
         <v>16</v>
@@ -3962,19 +4294,19 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="G20" s="0" t="n">
         <v>6</v>
@@ -4006,19 +4338,19 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="G21" s="0" t="n">
         <v>7</v>
@@ -4067,7 +4399,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="1" sqref="P61:P65 E3"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4082,32 +4414,32 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>14</v>
@@ -4115,66 +4447,66 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>